<commit_message>
Update Team Work Log with type of work
</commit_message>
<xml_diff>
--- a/Team Work Log.xlsx
+++ b/Team Work Log.xlsx
@@ -20,21 +20,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+  <si>
+    <t xml:space="preserve">Team Work Log</t>
+  </si>
   <si>
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Hours worked</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ryan Arnold</t>
   </si>
   <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Micah Smith</t>
   </si>
   <si>
     <t xml:space="preserve">Quentin Lintz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Management + Implementation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 1 Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of Work Types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 2 Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overall Total</t>
   </si>
 </sst>
 </file>
@@ -45,11 +81,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -65,6 +102,26 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -75,12 +132,54 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -109,7 +208,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -118,11 +217,55 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -143,58 +286,297 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="K20" activeCellId="0" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.4744897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="11.3418367346939"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
+    <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
-        <v>42971</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>0.5</v>
+        <v>42968</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
+        <v>42969</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
+        <v>42970</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <v>42971</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
         <v>42972</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="C7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="1" t="n">
         <v>2.5</v>
       </c>
+      <c r="G7" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="8" t="n">
+        <f aca="false">SUM(B3:B7)</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="8" t="n">
+        <f aca="false">SUM(D3:D7)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="8" t="n">
+        <f aca="false">SUM(F3:F7)</f>
+        <v>5</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="I8" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="n">
+        <v>42973</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="I9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="n">
+        <v>42974</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="G10" s="5"/>
+      <c r="I10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="n">
+        <v>42975</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="G11" s="5"/>
+      <c r="I11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="n">
+        <v>42976</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="G12" s="5"/>
+      <c r="I12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="n">
+        <v>42977</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="G13" s="5"/>
+      <c r="I13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="n">
+        <v>42978</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="G14" s="5"/>
+      <c r="I14" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="n">
+        <v>42979</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="n">
+        <f aca="false">SUM(B9:B15)</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="8" t="n">
+        <f aca="false">SUM(D9:D15)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="8" t="n">
+        <f aca="false">SUM(F9:F15)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="7"/>
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="n">
+        <v>42980</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="n">
+        <v>42981</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="n">
+        <v>42982</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="n">
+        <v>42983</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="n">
+        <v>42984</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="13" t="n">
+        <f aca="false">SUM(B16,B8,B17:B21)</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="13" t="n">
+        <f aca="false">SUM(D16,D8,D17:D21)</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="F22" s="13" t="n">
+        <f aca="false">SUM(F16,F8,F17:F21)</f>
+        <v>5</v>
+      </c>
+      <c r="G22" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added 3 windows: main menu, generate, and load
</commit_message>
<xml_diff>
--- a/Team Work Log.xlsx
+++ b/Team Work Log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t xml:space="preserve">Team Work Log</t>
   </si>
@@ -58,10 +58,10 @@
     <t xml:space="preserve">Implementation</t>
   </si>
   <si>
+    <t xml:space="preserve">Management</t>
+  </si>
+  <si>
     <t xml:space="preserve">Testing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Management</t>
   </si>
   <si>
     <t xml:space="preserve">Environment</t>
@@ -289,17 +289,18 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K20" activeCellId="0" sqref="K20"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.4744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.219387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -425,7 +426,12 @@
       </c>
       <c r="C9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="G9" s="5"/>
+      <c r="F9" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="I9" s="1" t="s">
         <v>6</v>
       </c>
@@ -447,7 +453,12 @@
       </c>
       <c r="C11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="G11" s="5"/>
+      <c r="F11" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
@@ -460,7 +471,7 @@
       <c r="E12" s="4"/>
       <c r="G12" s="5"/>
       <c r="I12" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -471,7 +482,7 @@
       <c r="E13" s="4"/>
       <c r="G13" s="5"/>
       <c r="I13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -509,7 +520,7 @@
       <c r="E16" s="9"/>
       <c r="F16" s="8" t="n">
         <f aca="false">SUM(F9:F15)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16" s="7"/>
       <c r="I16" s="11"/>
@@ -570,7 +581,7 @@
       <c r="E22" s="14"/>
       <c r="F22" s="13" t="n">
         <f aca="false">SUM(F16,F8,F17:F21)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G22" s="12"/>
     </row>

</xml_diff>

<commit_message>
Finished loading file part of UI and updated the input CSVs with a participation column
</commit_message>
<xml_diff>
--- a/Team Work Log.xlsx
+++ b/Team Work Log.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t xml:space="preserve">Team Work Log</t>
   </si>
@@ -289,7 +289,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -480,7 +480,12 @@
       </c>
       <c r="C13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="G13" s="5"/>
+      <c r="F13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="I13" s="1" t="s">
         <v>12</v>
       </c>
@@ -520,7 +525,7 @@
       <c r="E16" s="9"/>
       <c r="F16" s="8" t="n">
         <f aca="false">SUM(F9:F15)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G16" s="7"/>
       <c r="I16" s="11"/>
@@ -581,7 +586,7 @@
       <c r="E22" s="14"/>
       <c r="F22" s="13" t="n">
         <f aca="false">SUM(F16,F8,F17:F21)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G22" s="12"/>
     </row>

</xml_diff>

<commit_message>
Finished Meet and List panels.
</commit_message>
<xml_diff>
--- a/Team Work Log.xlsx
+++ b/Team Work Log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -227,9 +227,6 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -280,6 +277,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -564,32 +564,32 @@
   <dimension ref="A1:AMK22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" style="2"/>
-    <col min="2" max="2" width="10.81640625" style="2"/>
-    <col min="3" max="3" width="12.90625" style="18" customWidth="1"/>
-    <col min="4" max="5" width="10.81640625" style="2"/>
-    <col min="6" max="6" width="12.1796875" style="2"/>
-    <col min="7" max="7" width="13.08984375" style="2"/>
-    <col min="8" max="8" width="10.81640625" style="2"/>
-    <col min="9" max="9" width="18.08984375" style="2"/>
-    <col min="10" max="1025" width="10.81640625" style="2"/>
+    <col min="1" max="1" width="14" style="1"/>
+    <col min="2" max="2" width="10.81640625" style="1"/>
+    <col min="3" max="3" width="12.90625" style="17" customWidth="1"/>
+    <col min="4" max="5" width="10.81640625" style="1"/>
+    <col min="6" max="6" width="12.1796875" style="1"/>
+    <col min="7" max="7" width="13.08984375" style="1"/>
+    <col min="8" max="8" width="10.81640625" style="1"/>
+    <col min="9" max="9" width="18.08984375" style="1"/>
+    <col min="10" max="1025" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
@@ -1609,25 +1609,25 @@
       <c r="AMJ1"/>
     </row>
     <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="H2"/>
@@ -2649,21 +2649,21 @@
       <c r="AMJ2"/>
     </row>
     <row r="3" spans="1:1024" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>42968</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>5.66</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D3"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="2">
+      <c r="E3" s="3"/>
+      <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H3"/>
@@ -3685,17 +3685,17 @@
       <c r="AMJ3"/>
     </row>
     <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>42969</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>0</v>
       </c>
-      <c r="C4" s="15"/>
+      <c r="C4" s="14"/>
       <c r="D4"/>
-      <c r="E4" s="4"/>
+      <c r="E4" s="3"/>
       <c r="F4"/>
-      <c r="G4" s="5"/>
+      <c r="G4" s="4"/>
       <c r="H4"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -4715,19 +4715,19 @@
       <c r="AMJ4"/>
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>42970</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="14"/>
       <c r="D5"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="2">
+      <c r="E5" s="3"/>
+      <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H5"/>
@@ -5749,19 +5749,19 @@
       <c r="AMJ5"/>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>42971</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="14"/>
       <c r="D6"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="2">
+      <c r="E6" s="3"/>
+      <c r="F6" s="1">
         <v>0.5</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H6"/>
@@ -6783,19 +6783,19 @@
       <c r="AMJ6"/>
     </row>
     <row r="7" spans="1:1024" ht="25" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>42972</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="14"/>
       <c r="D7"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="2">
+      <c r="E7" s="3"/>
+      <c r="F7" s="1">
         <v>2.5</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="H7"/>
@@ -7817,26 +7817,26 @@
       <c r="AMJ7"/>
     </row>
     <row r="8" spans="1:1024" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <f>SUM(B3:B7)</f>
         <v>5.66</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="8">
+      <c r="C8" s="15"/>
+      <c r="D8" s="7">
         <f>SUM(D3:D7)</f>
         <v>0</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="8">
+      <c r="E8" s="8"/>
+      <c r="F8" s="7">
         <f>SUM(F3:F7)</f>
         <v>5</v>
       </c>
-      <c r="G8" s="7"/>
+      <c r="G8" s="6"/>
       <c r="H8"/>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J8"/>
@@ -8856,23 +8856,23 @@
       <c r="AMJ8"/>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>42973</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>0</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="14"/>
       <c r="D9"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="2">
+      <c r="E9" s="3"/>
+      <c r="F9" s="1">
         <v>1.5</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H9"/>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J9"/>
@@ -9892,19 +9892,19 @@
       <c r="AMJ9"/>
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>42974</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>0</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="14"/>
       <c r="D10"/>
-      <c r="E10" s="4"/>
+      <c r="E10" s="3"/>
       <c r="F10"/>
-      <c r="G10" s="5"/>
+      <c r="G10" s="4"/>
       <c r="H10"/>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J10"/>
@@ -10924,25 +10924,25 @@
       <c r="AMJ10"/>
     </row>
     <row r="11" spans="1:1024" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>42975</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>1.83</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>18</v>
       </c>
       <c r="D11"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="2">
+      <c r="E11" s="3"/>
+      <c r="F11" s="1">
         <v>0.5</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H11"/>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J11"/>
@@ -11962,19 +11962,19 @@
       <c r="AMJ11"/>
     </row>
     <row r="12" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>42976</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>0</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="14"/>
       <c r="D12"/>
-      <c r="E12" s="4"/>
+      <c r="E12" s="3"/>
       <c r="F12"/>
-      <c r="G12" s="5"/>
+      <c r="G12" s="4"/>
       <c r="H12"/>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J12"/>
@@ -12994,25 +12994,25 @@
       <c r="AMJ12"/>
     </row>
     <row r="13" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>42977</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>1.95</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D13"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="2">
+      <c r="E13" s="3"/>
+      <c r="F13" s="1">
         <v>3.5</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H13"/>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J13"/>
@@ -14032,19 +14032,19 @@
       <c r="AMJ13"/>
     </row>
     <row r="14" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>42978</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>0</v>
       </c>
-      <c r="C14" s="15"/>
+      <c r="C14" s="14"/>
       <c r="D14"/>
-      <c r="E14" s="4"/>
+      <c r="E14" s="3"/>
       <c r="F14"/>
-      <c r="G14" s="5"/>
+      <c r="G14" s="4"/>
       <c r="H14"/>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="10" t="s">
         <v>13</v>
       </c>
       <c r="J14"/>
@@ -15064,19 +15064,19 @@
       <c r="AMJ14"/>
     </row>
     <row r="15" spans="1:1024" ht="23" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>42979</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>4.5</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D15"/>
-      <c r="E15" s="4"/>
+      <c r="E15" s="3"/>
       <c r="F15"/>
-      <c r="G15" s="5"/>
+      <c r="G15" s="4"/>
       <c r="H15"/>
       <c r="I15"/>
       <c r="J15"/>
@@ -16095,41 +16095,41 @@
       <c r="AMI15"/>
       <c r="AMJ15"/>
     </row>
-    <row r="16" spans="1:1024" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:1024" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="7">
         <f>SUM(B9:B15)</f>
         <v>8.2800000000000011</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="8">
+      <c r="C16" s="15"/>
+      <c r="D16" s="7">
         <f>SUM(D9:D15)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="8">
+      <c r="E16" s="8"/>
+      <c r="F16" s="7">
         <f>SUM(F9:F15)</f>
         <v>5.5</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="I16" s="11"/>
+      <c r="G16" s="6"/>
+      <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:1024" ht="23" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>42980</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>4.5</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>20</v>
       </c>
       <c r="D17"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="3"/>
       <c r="F17"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="4"/>
       <c r="H17"/>
       <c r="I17"/>
       <c r="J17"/>
@@ -17148,15 +17148,20 @@
       <c r="AMI17"/>
       <c r="AMJ17"/>
     </row>
-    <row r="18" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+    <row r="18" spans="1:1024" ht="23" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>42981</v>
       </c>
-      <c r="C18" s="15"/>
+      <c r="B18" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>20</v>
+      </c>
       <c r="D18"/>
-      <c r="E18" s="4"/>
+      <c r="E18" s="3"/>
       <c r="F18"/>
-      <c r="G18" s="5"/>
+      <c r="G18" s="4"/>
       <c r="H18"/>
       <c r="I18"/>
       <c r="J18"/>
@@ -18176,14 +18181,14 @@
       <c r="AMJ18"/>
     </row>
     <row r="19" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>42982</v>
       </c>
-      <c r="C19" s="15"/>
+      <c r="C19" s="14"/>
       <c r="D19"/>
-      <c r="E19" s="4"/>
+      <c r="E19" s="3"/>
       <c r="F19"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="4"/>
       <c r="H19"/>
       <c r="I19"/>
       <c r="J19"/>
@@ -19203,14 +19208,14 @@
       <c r="AMJ19"/>
     </row>
     <row r="20" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>42983</v>
       </c>
-      <c r="C20" s="15"/>
+      <c r="C20" s="14"/>
       <c r="D20"/>
-      <c r="E20" s="4"/>
+      <c r="E20" s="3"/>
       <c r="F20"/>
-      <c r="G20" s="5"/>
+      <c r="G20" s="4"/>
       <c r="H20"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -20230,14 +20235,14 @@
       <c r="AMJ20"/>
     </row>
     <row r="21" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>42984</v>
       </c>
-      <c r="C21" s="15"/>
+      <c r="C21" s="14"/>
       <c r="D21"/>
-      <c r="E21" s="4"/>
+      <c r="E21" s="3"/>
       <c r="F21"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="4"/>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21"/>
@@ -21256,25 +21261,25 @@
       <c r="AMI21"/>
       <c r="AMJ21"/>
     </row>
-    <row r="22" spans="1:1024" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="12" t="s">
+    <row r="22" spans="1:1024" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="12">
         <f>SUM(B16,B8,B17:B21)</f>
-        <v>18.440000000000001</v>
+        <v>18.940000000000001</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="13">
+      <c r="C22" s="16"/>
+      <c r="D22" s="12">
         <f>SUM(D16,D8,D17:D21)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="13">
+      <c r="E22" s="13"/>
+      <c r="F22" s="12">
         <f>SUM(F16,F8,F17:F21)</f>
         <v>10.5</v>
       </c>
-      <c r="G22" s="12"/>
+      <c r="G22" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added ability to add a participant
</commit_message>
<xml_diff>
--- a/Team Work Log.xlsx
+++ b/Team Work Log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t xml:space="preserve">Team Work Log (in hours)</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">Requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirements + Environment</t>
   </si>
   <si>
     <t xml:space="preserve">Design</t>
@@ -329,21 +332,22 @@
   </sheetPr>
   <dimension ref="1:22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.219387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.7091836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.015306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4480,7 +4484,7 @@
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="25.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
         <v>42970</v>
       </c>
@@ -4491,10 +4495,10 @@
       <c r="D5" s="0"/>
       <c r="E5" s="6"/>
       <c r="F5" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>7</v>
+      <c r="G5" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="H5" s="0"/>
       <c r="I5" s="0"/>
@@ -5528,7 +5532,7 @@
         <v>0.5</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H6" s="0"/>
       <c r="I6" s="0"/>
@@ -6562,7 +6566,7 @@
         <v>2.5</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H7" s="0"/>
       <c r="I7" s="0"/>
@@ -7584,7 +7588,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="10" t="n">
         <f aca="false">SUM(B3:B7)</f>
@@ -7598,12 +7602,12 @@
       <c r="E8" s="12"/>
       <c r="F8" s="10" t="n">
         <f aca="false">SUM(F3:F7)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="0"/>
       <c r="I8" s="13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J8" s="0"/>
       <c r="K8" s="0"/>
@@ -8635,7 +8639,7 @@
         <v>1.5</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H9" s="0"/>
       <c r="I9" s="1" t="s">
@@ -9671,7 +9675,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="0"/>
       <c r="I10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J10" s="0"/>
       <c r="K10" s="0"/>
@@ -10697,7 +10701,7 @@
         <v>1.83</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D11" s="0"/>
       <c r="E11" s="6"/>
@@ -10705,11 +10709,11 @@
         <v>0.5</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H11" s="0"/>
       <c r="I11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J11" s="0"/>
       <c r="K11" s="0"/>
@@ -11741,7 +11745,7 @@
       <c r="G12" s="7"/>
       <c r="H12" s="0"/>
       <c r="I12" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J12" s="0"/>
       <c r="K12" s="0"/>
@@ -12767,7 +12771,7 @@
         <v>1.95</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" s="0"/>
       <c r="E13" s="6"/>
@@ -12775,11 +12779,11 @@
         <v>3.5</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H13" s="0"/>
       <c r="I13" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J13" s="0"/>
       <c r="K13" s="0"/>
@@ -13811,7 +13815,7 @@
       <c r="G14" s="7"/>
       <c r="H14" s="0"/>
       <c r="I14" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J14" s="0"/>
       <c r="K14" s="0"/>
@@ -14837,7 +14841,7 @@
         <v>4.5</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D15" s="0"/>
       <c r="E15" s="6"/>
@@ -14845,7 +14849,7 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H15" s="0"/>
       <c r="I15" s="0"/>
@@ -15867,7 +15871,7 @@
     </row>
     <row r="16" s="10" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="10" t="n">
         <f aca="false">SUM(B9:B15)</f>
@@ -15894,10 +15898,11 @@
         <v>4.5</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D17" s="0"/>
       <c r="E17" s="6"/>
+      <c r="F17" s="0"/>
       <c r="G17" s="7"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
@@ -16925,7 +16930,7 @@
         <v>0.5</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D18" s="0"/>
       <c r="E18" s="6"/>
@@ -16933,7 +16938,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H18" s="0"/>
       <c r="I18" s="0"/>
@@ -17953,7 +17958,7 @@
       <c r="AMI18" s="0"/>
       <c r="AMJ18" s="0"/>
     </row>
-    <row r="19" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="n">
         <v>42982</v>
       </c>
@@ -17961,8 +17966,12 @@
       <c r="C19" s="5"/>
       <c r="D19" s="0"/>
       <c r="E19" s="6"/>
-      <c r="F19" s="0"/>
-      <c r="G19" s="7"/>
+      <c r="F19" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="H19" s="0"/>
       <c r="I19" s="0"/>
       <c r="J19" s="0"/>
@@ -21039,7 +21048,7 @@
     </row>
     <row r="22" s="10" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="16" t="n">
         <f aca="false">SUM(B16,B8,B17:B21)</f>
@@ -21053,7 +21062,7 @@
       <c r="E22" s="18"/>
       <c r="F22" s="16" t="n">
         <f aca="false">SUM(F16,F8,F17:F21)</f>
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G22" s="15"/>
     </row>

</xml_diff>